<commit_message>
fixed my own bugs <3
</commit_message>
<xml_diff>
--- a/Experiments/221227_Mdh/buffers-mt.xlsx
+++ b/Experiments/221227_Mdh/buffers-mt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryancardiff/Documents/GitHub/WHISPR/Experiments/221227_Mdh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8F02E4-5FB9-AD48-860B-11B0D9CBACC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB51A817-02BF-1B44-94DF-5F499FB5A338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Biotin</t>
   </si>
@@ -73,18 +73,6 @@
   </si>
   <si>
     <t>Pyruvate</t>
-  </si>
-  <si>
-    <t>mdh_2.5</t>
-  </si>
-  <si>
-    <t>mdh_1</t>
-  </si>
-  <si>
-    <t>mdh_.2</t>
-  </si>
-  <si>
-    <t>mdh_0</t>
   </si>
   <si>
     <t>std_100</t>
@@ -388,7 +376,7 @@
   <dimension ref="A1:T993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -405,7 +393,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -444,21 +432,21 @@
         <v>11</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -504,7 +492,7 @@
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -550,7 +538,7 @@
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
@@ -596,7 +584,7 @@
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
@@ -642,7 +630,7 @@
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2"/>
       <c r="D6" s="2"/>
@@ -669,7 +657,7 @@
     </row>
     <row r="7" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2"/>
       <c r="D7" s="2"/>
@@ -723,7 +711,7 @@
     </row>
     <row r="9" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2"/>
       <c r="D9" s="2"/>

</xml_diff>